<commit_message>
Added test cases for v2
</commit_message>
<xml_diff>
--- a/Tokenizing/tokenizing_test_cases.xlsx
+++ b/Tokenizing/tokenizing_test_cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/GitCPR/2022-CPR101-NII-Group-01-Project/Tokenizing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54DC09D-1132-4F48-BC1C-0A6E39D5B2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302EF756-F307-DE4D-99B3-FAA95432FD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
           <rPr>
             <b/>
             <sz val="12"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -96,8 +96,9 @@
         <r>
           <rPr>
             <sz val="12"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> means a positive test expecting a successful result.
 </t>
@@ -106,7 +107,7 @@
           <rPr>
             <b/>
             <sz val="12"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -115,14 +116,15 @@
         <r>
           <rPr>
             <sz val="12"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> means a negative test to generate a validation message or explore unexpected, undefined behaviours.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{E121AF1F-0408-4713-A265-1FEF41AD73A9}">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{E121AF1F-0408-4713-A265-1FEF41AD73A9}">
       <text>
         <r>
           <rPr>
@@ -168,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>Program
 or module:</t>
@@ -446,12 +448,78 @@
   <si>
     <t>Version 3</t>
   </si>
+  <si>
+    <t>Sebastian Rubina 08/APR/2022</t>
+  </si>
+  <si>
+    <t>1st, 2nd phrase, The third phrase, This is 4th phrase, This is the 5th phrase</t>
+  </si>
+  <si>
+    <t>Phrase $1 is '1st'
+Phrase $2 is ' 2nd phrase'
+Phrase $3 is ' The third phrase'
+Phrase $4 is ' This is 4th phrase'
+Phrase $5 is ' This is the 5th phrase'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputed series of phrases (5 phrases) of different lenghts (1 word, 2 words, 3 words, 4 words and 5 words respectively). Worked as expected. </t>
+  </si>
+  <si>
+    <t>+ Tested 5 phrases of different lenghts</t>
+  </si>
+  <si>
+    <t>+ Tested pressing enter without inputting anything</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressed enter with no inputs, program just prompted the user again for phrases, worked as intended and expected. </t>
+  </si>
+  <si>
+    <t>+ Tested three very long phrases (200+ characters)</t>
+  </si>
+  <si>
+    <t>200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ , 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ , 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+</t>
+  </si>
+  <si>
+    <t>Phrase $1 is '200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ '
+Phrase $2 is ' 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ '
+Phrase $3 is ' 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ 200+ '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputed 3 very long (200+ characters) phrases, separated by commas, worked as intended, gave the output that I was expecting. </t>
+  </si>
+  <si>
+    <t>This is a test comma \, and this is another phrase,</t>
+  </si>
+  <si>
+    <t>+ Inputted a backslash before a comma to see if it would break the code and not separate it</t>
+  </si>
+  <si>
+    <t>Phrase $1 is 'This is a test comma \'
+Phrase $2 is ' and this is another phrase'</t>
+  </si>
+  <si>
+    <t>Worked as intended, the backslash didn't affect the comma and it still divided the phrases by the comma</t>
+  </si>
+  <si>
+    <t>+ Inputted spaces between commas with nothing else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, , , </t>
+  </si>
+  <si>
+    <t>Phrase $1 is ' '
+Phrase $2 is ' '
+Phrase $3 is ' '</t>
+  </si>
+  <si>
+    <t>Worked as expected, divided the phrases into different phrases by the comma</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -519,6 +587,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -546,7 +634,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -807,6 +895,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -815,7 +916,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -939,6 +1040,24 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1224,24 +1343,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="29.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.1" thickBot="1">
+    <row r="1" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1373,7 @@
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:9" s="18" customFormat="1" ht="35.25" customHeight="1" thickBot="1">
+    <row r="2" spans="1:9" s="18" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
         <v>2</v>
       </c>
@@ -1269,7 +1388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="19" customFormat="1" ht="24" customHeight="1" thickBot="1">
+    <row r="3" spans="1:9" s="19" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>5</v>
       </c>
@@ -1293,7 +1412,7 @@
       </c>
       <c r="I3" s="25"/>
     </row>
-    <row r="4" spans="1:9" ht="113.1" customHeight="1">
+    <row r="4" spans="1:9" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
@@ -1315,7 +1434,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="409.6">
+    <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
@@ -1338,7 +1457,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="409.6">
+    <row r="6" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
@@ -1363,7 +1482,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="56.1">
+    <row r="7" spans="1:9" ht="56" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
@@ -1384,7 +1503,7 @@
       <c r="H7" s="30"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="210.95" thickBot="1">
+    <row r="8" spans="1:9" ht="211" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>12</v>
       </c>
@@ -1409,7 +1528,7 @@
       <c r="H8" s="30"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" s="18" customFormat="1" ht="35.25" customHeight="1" thickBot="1">
+    <row r="9" spans="1:9" s="18" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
         <v>35</v>
       </c>
@@ -1421,14 +1540,14 @@
         <v>3</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="19" customFormat="1" ht="24" customHeight="1" thickBot="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="19" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="43" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="23" t="s">
@@ -1448,106 +1567,162 @@
       </c>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:9" ht="15.95">
-      <c r="A11" s="5"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+    <row r="11" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>42</v>
+      </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="46" t="s">
+        <v>43</v>
+      </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="15.95">
-      <c r="A12" s="5"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
+    <row r="12" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="42"/>
       <c r="D12" s="11"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="46" t="s">
+        <v>46</v>
+      </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="15.95">
-      <c r="A13" s="5"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+    <row r="13" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>49</v>
+      </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="3"/>
+      <c r="F13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>50</v>
+      </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="15.95">
-      <c r="A14" s="5"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+    <row r="14" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>53</v>
+      </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="3"/>
+      <c r="F14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="46" t="s">
+        <v>54</v>
+      </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="15.95">
-      <c r="A15" s="5"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+    <row r="15" spans="1:9" ht="43" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>57</v>
+      </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="3"/>
+      <c r="F15" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="46" t="s">
+        <v>58</v>
+      </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="17.100000000000001" thickBot="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" ht="35.25" customHeight="1" thickBot="1">
-      <c r="A17" s="40" t="s">
+    <row r="16" spans="1:9" s="18" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="28" t="s">
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G16" s="29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="19" customFormat="1" ht="24" customHeight="1" thickBot="1">
-      <c r="A18" s="21" t="s">
+    <row r="17" spans="1:9" s="19" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B17" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C17" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F17" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G17" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="25"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.95">
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A18" s="5"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" s="5"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
@@ -1557,7 +1732,7 @@
       <c r="G19" s="3"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="15.95">
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" s="5"/>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
@@ -1567,7 +1742,7 @@
       <c r="G20" s="3"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="15.95">
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" s="5"/>
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
@@ -1577,7 +1752,7 @@
       <c r="G21" s="3"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="15.95">
+    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" s="5"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
@@ -1587,7 +1762,7 @@
       <c r="G22" s="3"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="15.95">
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" s="5"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -1597,7 +1772,7 @@
       <c r="G23" s="3"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="15.95">
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" s="5"/>
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
@@ -1607,7 +1782,7 @@
       <c r="G24" s="3"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="15.95">
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="5"/>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
@@ -1617,31 +1792,21 @@
       <c r="G25" s="3"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="15.95">
-      <c r="A26" s="5"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" ht="17.100000000000001" thickBot="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="4"/>
+    <row r="26" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="4"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A16:E16"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1652,21 +1817,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007DA71BB3427D8A4D8C6B1D9FC83B8523" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff806a6af6c9da5df570eefd46bafc37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="871f9c32-6190-4c20-b083-b734e08baf9d" xmlns:ns3="f9e5404a-8fb4-4d07-81e3-37a7278de386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="91c5258a233d7e8320f07641405ff8a3" ns2:_="" ns3:_="">
     <xsd:import namespace="871f9c32-6190-4c20-b083-b734e08baf9d"/>
@@ -1883,14 +2033,53 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3825A01-A6C5-4DDF-BA11-8EF1674108E8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90A86611-893E-47D5-A227-D1AFE198ACA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="871f9c32-6190-4c20-b083-b734e08baf9d"/>
+    <ds:schemaRef ds:uri="f9e5404a-8fb4-4d07-81e3-37a7278de386"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E0EFC20-9D0E-4ED7-BF9B-D6EADFF35E7A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E0EFC20-9D0E-4ED7-BF9B-D6EADFF35E7A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90A86611-893E-47D5-A227-D1AFE198ACA8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3825A01-A6C5-4DDF-BA11-8EF1674108E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>